<commit_message>
Ajout d'une ligne dans le cahier des charges
</commit_message>
<xml_diff>
--- a/Cahier des charges.xlsx
+++ b/Cahier des charges.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10313"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25028"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/corentin/UTBM/BR02/IR5/IR5A-B-P2022/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\UTBM\COURS\BR3\IR5A-B-P2022\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{45B9719F-4820-FF4F-B54C-E82759073E64}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63D098AE-3FAC-4455-ADF8-BBEE921E9620}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="16080" xr2:uid="{B19E6B91-1F07-134E-9E4D-5B55020B3C38}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{B19E6B91-1F07-134E-9E4D-5B55020B3C38}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="32">
   <si>
     <t>Fonction</t>
   </si>
@@ -125,6 +125,12 @@
   </si>
   <si>
     <t>(pour les persos je pense qu'il y a des aspects que je ne connais pas)</t>
+  </si>
+  <si>
+    <t>Accentuer l'immersion dans la partie</t>
+  </si>
+  <si>
+    <t>Cacher un maximum les interfaces, préférer des raccourcis ou des actions simples à la souris</t>
   </si>
 </sst>
 </file>
@@ -479,20 +485,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9554EB17-89ED-C64B-9BBF-CEAEFCF9A894}">
-  <dimension ref="A1:F13"/>
+  <dimension ref="A1:F14"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="136" workbookViewId="0">
-      <selection activeCell="A14" sqref="A14"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="136" workbookViewId="0">
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.796875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="50.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="89.83203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="16384" width="10.83203125" style="1"/>
+    <col min="1" max="1" width="50.296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="89.796875" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="16384" width="10.796875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -509,7 +515,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>4</v>
       </c>
@@ -523,7 +529,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>10</v>
       </c>
@@ -537,7 +543,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>11</v>
       </c>
@@ -551,7 +557,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>14</v>
       </c>
@@ -562,7 +568,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>16</v>
       </c>
@@ -573,7 +579,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>27</v>
       </c>
@@ -584,7 +590,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>19</v>
       </c>
@@ -595,7 +601,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>21</v>
       </c>
@@ -606,7 +612,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>23</v>
       </c>
@@ -617,7 +623,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>25</v>
       </c>
@@ -628,9 +634,20 @@
         <v>6</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
         <v>29</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A14" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>